<commit_message>
added time taken for indexed db
</commit_message>
<xml_diff>
--- a/project_deliverables/runtime.xlsx
+++ b/project_deliverables/runtime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="440" windowWidth="25440" windowHeight="14240" xr2:uid="{17C89B23-6EE6-5B4E-8BE3-6BF3D69AE5CD}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14240" xr2:uid="{17C89B23-6EE6-5B4E-8BE3-6BF3D69AE5CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Query</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t xml:space="preserve">Quarter size </t>
+  </si>
+  <si>
+    <t>Full size /w index</t>
   </si>
 </sst>
 </file>
@@ -415,28 +418,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1908773B-D8FD-8A44-BB68-27C89FA808DE}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -444,13 +449,16 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -458,13 +466,16 @@
         <v>4154.3940000000002</v>
       </c>
       <c r="C3">
+        <v>3125.2950000000001</v>
+      </c>
+      <c r="D3">
         <v>1662.4059999999999</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>127.783</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -472,13 +483,16 @@
         <v>2541.451</v>
       </c>
       <c r="C4">
+        <v>230.09100000000001</v>
+      </c>
+      <c r="D4">
         <v>1834.18</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>138.15199999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -486,13 +500,16 @@
         <v>1570.3689999999999</v>
       </c>
       <c r="C5">
+        <v>94.924000000000007</v>
+      </c>
+      <c r="D5">
         <v>1247.038</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>375.65100000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -500,13 +517,16 @@
         <v>1426.471</v>
       </c>
       <c r="C6">
+        <v>5.1360000000000001</v>
+      </c>
+      <c r="D6">
         <v>1132.1130000000001</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>381.95100000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -514,13 +534,16 @@
         <v>3557.73</v>
       </c>
       <c r="C7">
+        <v>644.971</v>
+      </c>
+      <c r="D7">
         <v>1324.7349999999999</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>221.51499999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -528,13 +551,16 @@
         <v>3442.0169999999998</v>
       </c>
       <c r="C8">
+        <v>3008.6819999999998</v>
+      </c>
+      <c r="D8">
         <v>1424.2059999999999</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>613.28499999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -542,13 +568,16 @@
         <v>10311.703</v>
       </c>
       <c r="C9">
+        <v>11585.268</v>
+      </c>
+      <c r="D9">
         <v>4747.8680000000004</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1033.4559999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -556,13 +585,16 @@
         <v>4312.1229999999996</v>
       </c>
       <c r="C10">
+        <v>3373.23</v>
+      </c>
+      <c r="D10">
         <v>1256.6079999999999</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>597.80799999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -570,13 +602,16 @@
         <v>17211.909</v>
       </c>
       <c r="C11">
+        <v>26880.744999999999</v>
+      </c>
+      <c r="D11">
         <v>4555.3320000000003</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1811.76</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -584,13 +619,16 @@
         <v>5485.5450000000001</v>
       </c>
       <c r="C12">
+        <v>1646.471</v>
+      </c>
+      <c r="D12">
         <v>912.96100000000001</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>325.09800000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -598,13 +636,16 @@
         <v>3021.31</v>
       </c>
       <c r="C13">
+        <v>435.64699999999999</v>
+      </c>
+      <c r="D13">
         <v>510.35700000000003</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>229.773</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
@@ -612,13 +653,16 @@
         <v>26452.778999999999</v>
       </c>
       <c r="C14">
+        <v>16830.469000000001</v>
+      </c>
+      <c r="D14">
         <v>9045.098</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>4610.5259999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
@@ -626,13 +670,16 @@
         <v>10514.291999999999</v>
       </c>
       <c r="C15">
+        <v>1539.2619999999999</v>
+      </c>
+      <c r="D15">
         <v>2565.9989999999998</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>1364.6880000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>10</v>
       </c>
@@ -640,15 +687,18 @@
         <v>2415.11</v>
       </c>
       <c r="C16">
+        <v>518.20299999999997</v>
+      </c>
+      <c r="D16">
         <v>669.65200000000004</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>297.27499999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>